<commit_message>
chore: exporting results to desired file format
</commit_message>
<xml_diff>
--- a/extraction.xlsx
+++ b/extraction.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\made\charla-api-extraction-imob-fin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97587F7F-08EA-4A20-9682-33804799BB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -307,8 +313,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,13 +377,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -415,7 +429,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -449,6 +463,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -483,9 +498,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -658,14 +674,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="157.28515625" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -684,7 +706,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -695,7 +717,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -706,7 +728,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -717,7 +739,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -728,7 +750,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -739,7 +761,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -750,7 +772,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -761,7 +783,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -772,7 +794,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -783,7 +805,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -794,7 +816,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -805,7 +827,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -816,7 +838,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -827,7 +849,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -838,7 +860,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -849,7 +871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -860,7 +882,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -871,7 +893,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -882,7 +904,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -893,7 +915,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -904,7 +926,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -915,7 +937,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -926,7 +948,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -937,7 +959,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -948,7 +970,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -959,7 +981,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -970,7 +992,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -981,7 +1003,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -992,7 +1014,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1003,7 +1025,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1014,7 +1036,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1025,7 +1047,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1036,7 +1058,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1047,7 +1069,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1058,7 +1080,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1069,7 +1091,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1080,7 +1102,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1091,7 +1113,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1102,7 +1124,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1113,7 +1135,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1124,7 +1146,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1135,7 +1157,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1146,7 +1168,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1157,7 +1179,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1168,7 +1190,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1179,7 +1201,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1190,7 +1212,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1201,7 +1223,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1212,7 +1234,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1223,7 +1245,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1234,7 +1256,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1245,7 +1267,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1256,7 +1278,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1267,7 +1289,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1278,7 +1300,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1289,7 +1311,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1300,7 +1322,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1311,7 +1333,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1322,7 +1344,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1333,7 +1355,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1344,7 +1366,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1355,7 +1377,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1366,7 +1388,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1377,7 +1399,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1388,7 +1410,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1399,7 +1421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1410,7 +1432,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1421,7 +1443,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1432,7 +1454,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1443,7 +1465,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1454,7 +1476,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1465,7 +1487,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1476,7 +1498,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1487,7 +1509,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1498,7 +1520,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1509,7 +1531,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1520,7 +1542,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1531,7 +1553,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1542,7 +1564,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1553,7 +1575,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1564,7 +1586,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1575,7 +1597,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1586,7 +1608,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1597,7 +1619,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1608,7 +1630,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -1619,7 +1641,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1630,7 +1652,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -1641,7 +1663,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -1652,7 +1674,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -1663,7 +1685,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -1674,7 +1696,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -1685,7 +1707,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -1696,7 +1718,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -1707,7 +1729,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -1718,7 +1740,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -1729,7 +1751,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -1740,7 +1762,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -1751,7 +1773,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -1762,7 +1784,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -1773,7 +1795,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -1784,7 +1806,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -1795,7 +1817,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -1806,7 +1828,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -1817,7 +1839,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -1828,7 +1850,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -1839,7 +1861,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -1850,7 +1872,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -1861,7 +1883,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -1872,7 +1894,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -1883,7 +1905,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -1894,7 +1916,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -1905,7 +1927,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -1916,7 +1938,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -1927,7 +1949,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -1938,7 +1960,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -1949,7 +1971,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>

</xml_diff>